<commit_message>
Update the main power switch
</commit_message>
<xml_diff>
--- a/Electrical/MainBoard/bom/bom_digikey_PIC32_1.xlsx
+++ b/Electrical/MainBoard/bom/bom_digikey_PIC32_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\Desktop\Robot\Electrical\MainBoard\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64B0396-2CB5-4A21-BF01-750082E9FD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB29FCF-6761-4AF8-8B5B-CB0AF51594BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8C1C06BF-AC5E-4C14-BE4D-7CA0470A3B8C}"/>
   </bookViews>
@@ -377,9 +377,6 @@
     <t>26-60-4040_MOL</t>
   </si>
   <si>
-    <t>708-3039-ND</t>
-  </si>
-  <si>
     <t>M1, M2</t>
   </si>
   <si>
@@ -644,12 +641,6 @@
     <t>OS102011MS2QN1</t>
   </si>
   <si>
-    <t>Bulgin</t>
-  </si>
-  <si>
-    <t>C1553PBNAW</t>
-  </si>
-  <si>
     <t>Phoenix Contact</t>
   </si>
   <si>
@@ -696,6 +687,15 @@
   </si>
   <si>
     <t>R1, R17, R27</t>
+  </si>
+  <si>
+    <t>E-Switch</t>
+  </si>
+  <si>
+    <t>RA83231100</t>
+  </si>
+  <si>
+    <t>EG5682-ND</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE472AD2-9AB7-4FBD-ACED-6AB892D95601}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1074,10 +1076,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
         <v>162</v>
-      </c>
-      <c r="E1" t="s">
-        <v>163</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1091,7 +1093,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1100,10 +1102,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
         <v>164</v>
-      </c>
-      <c r="E2" t="s">
-        <v>165</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1126,10 +1128,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1143,7 +1145,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -1152,10 +1154,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -1178,10 +1180,10 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -1204,10 +1206,10 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" t="s">
         <v>169</v>
-      </c>
-      <c r="E6" t="s">
-        <v>170</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -1230,10 +1232,10 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" t="s">
         <v>171</v>
-      </c>
-      <c r="E7" t="s">
-        <v>172</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -1256,10 +1258,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -1282,10 +1284,10 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" t="s">
         <v>174</v>
-      </c>
-      <c r="E9" t="s">
-        <v>175</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -1299,7 +1301,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
@@ -1308,10 +1310,10 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -1334,10 +1336,10 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -1351,7 +1353,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -1360,10 +1362,10 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -1386,10 +1388,10 @@
         <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -1412,10 +1414,10 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -1438,10 +1440,10 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -1464,10 +1466,10 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -1481,7 +1483,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
         <v>52</v>
@@ -1490,10 +1492,10 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" t="s">
         <v>183</v>
-      </c>
-      <c r="E17" t="s">
-        <v>184</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -1507,7 +1509,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s">
         <v>52</v>
@@ -1516,10 +1518,10 @@
         <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -1542,10 +1544,10 @@
         <v>58</v>
       </c>
       <c r="D19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
         <v>186</v>
-      </c>
-      <c r="E19" t="s">
-        <v>187</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -1568,7 +1570,7 @@
         <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -1594,7 +1596,7 @@
         <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E21" t="s">
         <v>65</v>
@@ -1620,7 +1622,7 @@
         <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E22" t="s">
         <v>69</v>
@@ -1646,7 +1648,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E23">
         <v>22232041</v>
@@ -1672,7 +1674,7 @@
         <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E24" t="s">
         <v>77</v>
@@ -1698,7 +1700,7 @@
         <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E25" t="s">
         <v>81</v>
@@ -1724,10 +1726,10 @@
         <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1750,10 +1752,10 @@
         <v>90</v>
       </c>
       <c r="D27" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" t="s">
         <v>195</v>
-      </c>
-      <c r="E27" t="s">
-        <v>196</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -1776,7 +1778,7 @@
         <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E28">
         <v>4628</v>
@@ -1802,7 +1804,7 @@
         <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E29">
         <v>22232021</v>
@@ -1828,7 +1830,7 @@
         <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E30">
         <v>22232021</v>
@@ -1854,10 +1856,10 @@
         <v>104</v>
       </c>
       <c r="D31" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" t="s">
         <v>198</v>
-      </c>
-      <c r="E31" t="s">
-        <v>199</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1880,10 +1882,10 @@
         <v>108</v>
       </c>
       <c r="D32" t="s">
+        <v>199</v>
+      </c>
+      <c r="E32" t="s">
         <v>200</v>
-      </c>
-      <c r="E32" t="s">
-        <v>201</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -1906,16 +1908,16 @@
         <v>112</v>
       </c>
       <c r="D33" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="E33" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>113</v>
+        <v>219</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -1923,16 +1925,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
         <v>114</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>115</v>
       </c>
-      <c r="C34" t="s">
-        <v>116</v>
-      </c>
       <c r="D34" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E34">
         <v>1890963</v>
@@ -1941,7 +1943,7 @@
         <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H34">
         <v>2</v>
@@ -1949,25 +1951,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" t="s">
         <v>118</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>119</v>
       </c>
-      <c r="C35" t="s">
-        <v>120</v>
-      </c>
       <c r="D35" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E35" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H35">
         <v>5</v>
@@ -1975,16 +1977,16 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" t="s">
         <v>122</v>
-      </c>
-      <c r="B36" t="s">
-        <v>123</v>
       </c>
       <c r="C36" t="s">
         <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E36">
         <v>22232031</v>
@@ -1993,7 +1995,7 @@
         <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H36">
         <v>3</v>
@@ -2001,25 +2003,25 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" t="s">
         <v>125</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>126</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>202</v>
+      </c>
+      <c r="E37" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
         <v>127</v>
-      </c>
-      <c r="D37" t="s">
-        <v>205</v>
-      </c>
-      <c r="E37" t="s">
-        <v>207</v>
-      </c>
-      <c r="F37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" t="s">
-        <v>128</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -2027,16 +2029,16 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" t="s">
         <v>129</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>130</v>
       </c>
-      <c r="C38" t="s">
-        <v>131</v>
-      </c>
       <c r="D38" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E38">
         <v>1017514</v>
@@ -2045,7 +2047,7 @@
         <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H38">
         <v>2</v>
@@ -2053,25 +2055,25 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" t="s">
         <v>133</v>
       </c>
-      <c r="B39" t="s">
-        <v>134</v>
-      </c>
       <c r="C39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
+        <v>202</v>
+      </c>
+      <c r="E39" t="s">
         <v>205</v>
       </c>
-      <c r="E39" t="s">
-        <v>208</v>
-      </c>
       <c r="F39" t="s">
         <v>8</v>
       </c>
       <c r="G39" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H39">
         <v>2</v>
@@ -2079,25 +2081,25 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" t="s">
         <v>135</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>136</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" t="s">
+        <v>208</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" t="s">
         <v>137</v>
-      </c>
-      <c r="D40" t="s">
-        <v>210</v>
-      </c>
-      <c r="E40" t="s">
-        <v>211</v>
-      </c>
-      <c r="F40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" t="s">
-        <v>138</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -2105,25 +2107,25 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" t="s">
         <v>139</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>140</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>209</v>
+      </c>
+      <c r="E41" t="s">
+        <v>210</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" t="s">
         <v>141</v>
-      </c>
-      <c r="D41" t="s">
-        <v>212</v>
-      </c>
-      <c r="E41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G41" t="s">
-        <v>142</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -2131,25 +2133,25 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" t="s">
         <v>143</v>
       </c>
-      <c r="B42" t="s">
-        <v>144</v>
-      </c>
       <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" t="s">
+        <v>209</v>
+      </c>
+      <c r="E42" t="s">
+        <v>210</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" t="s">
         <v>141</v>
-      </c>
-      <c r="D42" t="s">
-        <v>212</v>
-      </c>
-      <c r="E42" t="s">
-        <v>213</v>
-      </c>
-      <c r="F42" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" t="s">
-        <v>142</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -2157,25 +2159,25 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" t="s">
         <v>145</v>
       </c>
-      <c r="B43" t="s">
-        <v>146</v>
-      </c>
       <c r="C43" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E43" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F43" t="s">
         <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -2183,25 +2185,25 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" t="s">
         <v>147</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>148</v>
       </c>
-      <c r="C44" t="s">
-        <v>149</v>
-      </c>
       <c r="D44" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E44" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F44" t="s">
         <v>8</v>
       </c>
       <c r="G44" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -2209,25 +2211,25 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" t="s">
         <v>150</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>151</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
+        <v>215</v>
+      </c>
+      <c r="E45" t="s">
+        <v>150</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" t="s">
         <v>152</v>
-      </c>
-      <c r="D45" t="s">
-        <v>218</v>
-      </c>
-      <c r="E45" t="s">
-        <v>151</v>
-      </c>
-      <c r="F45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" t="s">
-        <v>153</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -2235,16 +2237,16 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" t="s">
         <v>154</v>
-      </c>
-      <c r="B46" t="s">
-        <v>155</v>
       </c>
       <c r="C46" t="s">
         <v>74</v>
       </c>
       <c r="D46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E46">
         <v>22232041</v>

</xml_diff>